<commit_message>
Created the DataProvider Util for the ExcelData that is used in the createjob api test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/PhoenixTestData.xlsx
+++ b/src/test/resources/testData/PhoenixTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/372fac067aba4504/Desktop/SDET With Jatin/RestAssured/PhoenixTestAutomationFramework/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC10482D019C470C5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{690FAF49-3034-468A-8965-B9460B60BF38}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC10482D019C470C5ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0E69214-BF14-441A-BA09-C1171A58043E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateJobTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -40,6 +41,129 @@
   </si>
   <si>
     <t>iameng</t>
+  </si>
+  <si>
+    <t>mst_service_location_id</t>
+  </si>
+  <si>
+    <t>mst_platform_id</t>
+  </si>
+  <si>
+    <t>mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t>mst_oem_id</t>
+  </si>
+  <si>
+    <t>customer__first_name</t>
+  </si>
+  <si>
+    <t>customer__last_name</t>
+  </si>
+  <si>
+    <t>customer__mobile_number</t>
+  </si>
+  <si>
+    <t>customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t>customer__email_id</t>
+  </si>
+  <si>
+    <t>customer__email_id_alt</t>
+  </si>
+  <si>
+    <t>customer_address__flat_number</t>
+  </si>
+  <si>
+    <t>customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t>customer_address__street_name</t>
+  </si>
+  <si>
+    <t>customer_address__landmark</t>
+  </si>
+  <si>
+    <t>customer_address__area</t>
+  </si>
+  <si>
+    <t>customer_address__pincode</t>
+  </si>
+  <si>
+    <t>customer_address__country</t>
+  </si>
+  <si>
+    <t>customer_address__state</t>
+  </si>
+  <si>
+    <t>customer_product__dop</t>
+  </si>
+  <si>
+    <t>customer_product__serial_number</t>
+  </si>
+  <si>
+    <t>customer_product__imei1</t>
+  </si>
+  <si>
+    <t>customer_product__imei2</t>
+  </si>
+  <si>
+    <t>customer_product__popurl</t>
+  </si>
+  <si>
+    <t>customer_product__product_id</t>
+  </si>
+  <si>
+    <t>customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t>problems__id</t>
+  </si>
+  <si>
+    <t>problems__remark</t>
+  </si>
+  <si>
+    <t>Hilda</t>
+  </si>
+  <si>
+    <t>Sipes</t>
+  </si>
+  <si>
+    <t>512-517-3023</t>
+  </si>
+  <si>
+    <t>Nakia87@hotmail.com</t>
+  </si>
+  <si>
+    <t>Swamy nagar</t>
+  </si>
+  <si>
+    <t>61638 Graham Passage</t>
+  </si>
+  <si>
+    <t>Near Shivalayam</t>
+  </si>
+  <si>
+    <t>Kakinada</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>2025-09-30T18:30:00.000Z</t>
+  </si>
+  <si>
+    <t>over heat</t>
+  </si>
+  <si>
+    <t>12345700000000</t>
+  </si>
+  <si>
+    <t>96257600000000</t>
   </si>
 </sst>
 </file>
@@ -75,8 +199,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -400,4 +526,190 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76E6747-0BF4-4A15-9FFE-B69175D783C6}">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" customWidth="1"/>
+    <col min="19" max="19" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2">
+        <v>5125173023</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2">
+        <v>768</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2">
+        <v>516</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>6</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>